<commit_message>
Added some questions and suggestions in Progress
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -274,7 +274,9 @@
     <t>- Във вофрмата за записване да имаме текст със същия цвят като фона (т.е. невидим) от типа: дарявам си бъбрека и т.н.
 - Да направим някакъв измислен "форум", с който да наблъскаме тъпи въпроси и още по-некадърни отговори.
 - Да се избъзикаме с дължината на лекциите на Наков.
-- Да се избъзикаме с минималното количество жени.</t>
+- Да се избъзикаме с минималното количество жени.
+- Сайтът на български или на английски да е? Или да преведем контента?
+- Да измислим главните менюта - За нас, Начало, Контакти, Форум (с глупости в него)?, Обучения, Партньори, Форма за записване и вход, да направим имейл, на който да пращаме съобщения от контакт формата?;</t>
   </si>
 </sst>
 </file>
@@ -491,6 +493,10 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -509,15 +515,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -820,13 +822,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -842,11 +844,11 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -1276,12 +1278,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -1370,16 +1372,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:2" s="26" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="33"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="25">
@@ -1390,30 +1392,30 @@
       </c>
     </row>
     <row r="4" spans="1:2" s="26" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="31"/>
+      <c r="B4" s="33"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2" s="26" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="31"/>
+      <c r="B6" s="33"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
       <c r="B7" s="16"/>
     </row>
     <row r="8" spans="1:2" s="26" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="33"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="25">
@@ -1451,12 +1453,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -1601,34 +1603,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33" t="s">
+      <c r="D2" s="35"/>
+      <c r="E2" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="34" t="s">
+      <c r="F2" s="35"/>
+      <c r="G2" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="28" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1654,7 +1656,7 @@
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="16">
         <v>2</v>
       </c>
@@ -1672,7 +1674,7 @@
       <c r="G4" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="29" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added saint Nakov jpeg
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip Kolev\Documents\GitHub\Team-CedarChest\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8145" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
     <sheet name="Content" sheetId="3" r:id="rId5"/>
     <sheet name="Features" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -582,7 +577,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -617,7 +612,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -794,7 +789,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1265,7 +1260,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,8 +1581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
deleted useless tabs in progress.xlsx
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip Kolev\Documents\GitHub\Team-CedarChest\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8145" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8145" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="Deliverables" sheetId="2" r:id="rId2"/>
     <sheet name="Team contribution" sheetId="5" r:id="rId3"/>
     <sheet name="Assessment Criteria" sheetId="6" r:id="rId4"/>
-    <sheet name="Content" sheetId="3" r:id="rId5"/>
-    <sheet name="Features" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
   <si>
     <t>Assignement requirements</t>
   </si>
@@ -231,47 +234,6 @@
   </si>
   <si>
     <t>Team Contribution</t>
-  </si>
-  <si>
-    <t>Site name</t>
-  </si>
-  <si>
-    <t>Suggestion</t>
-  </si>
-  <si>
-    <t>Logo</t>
-  </si>
-  <si>
-    <t>http://f01.bis.bulcdn.net/fsh/6/9/2/6/e/65112/albums/5/b/3/32988/c/5/2/2204476.jpg?v=0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Navigation bar</t>
-  </si>
-  <si>
-    <t>http://css-tricks.com/</t>
-  </si>
-  <si>
-    <t>Сектор Смях</t>
-  </si>
-  <si>
-    <t>Хардуерен Университет "Св. Наков"</t>
-  </si>
-  <si>
-    <t>Motto</t>
-  </si>
-  <si>
-    <t>"За да ви е гадно!"</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>- Във вофрмата за записване да имаме текст със същия цвят като фона (т.е. невидим) от типа: дарявам си бъбрека и т.н.
-- Да направим някакъв измислен "форум", с който да наблъскаме тъпи въпроси и още по-некадърни отговори.
-- Да се избъзикаме с дължината на лекциите на Наков.
-- Да се избъзикаме с минималното количество жени.
-- Сайтът на български или на английски да е? Или да преведем контента?
-- Да измислим главните менюта - За нас, Начало, Контакти, Форум (с глупости в него)?, Обучения, Партньори, Форма за записване и вход, да направим имейл, на който да пращаме съобщения от контакт формата?;</t>
   </si>
 </sst>
 </file>
@@ -386,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -409,21 +371,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -487,11 +440,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -506,15 +454,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -789,7 +728,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -803,7 +742,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" sqref="A1:E2"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,13 +756,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -839,11 +778,11 @@
       <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -1260,7 +1199,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,12 +1212,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -1367,16 +1306,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:2" s="26" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="25">
@@ -1387,30 +1326,30 @@
       </c>
     </row>
     <row r="4" spans="1:2" s="26" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="33"/>
+      <c r="B4" s="30"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:2" s="26" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="30"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
       <c r="B7" s="16"/>
     </row>
     <row r="8" spans="1:2" s="26" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="33"/>
+      <c r="B8" s="30"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="25">
@@ -1436,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
@@ -1448,12 +1387,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
@@ -1575,225 +1514,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="77.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
-        <v>1</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="16">
-        <v>1</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="16">
-        <v>1</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
-        <v>2</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="16">
-        <v>2</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16">
-        <v>2</v>
-      </c>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
-        <v>3</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16">
-        <v>3</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16">
-        <v>3</v>
-      </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
-        <v>4</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16">
-        <v>4</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16">
-        <v>4</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
-        <v>5</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16">
-        <v>5</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16">
-        <v>5</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
-        <v>6</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16">
-        <v>6</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16">
-        <v>6</v>
-      </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
-        <v>7</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16">
-        <v>7</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16">
-        <v>7</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
-        <v>8</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16">
-        <v>8</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16">
-        <v>8</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed application form responsiveness
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8145" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8145" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
   <si>
     <t>Assignement requirements</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>Team Contribution</t>
+  </si>
+  <si>
+    <t>Fil</t>
   </si>
 </sst>
 </file>
@@ -310,7 +313,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,6 +350,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -376,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -454,6 +463,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -739,7 +751,7 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
@@ -831,7 +843,7 @@
       <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="32" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="8"/>
@@ -859,7 +871,7 @@
       <c r="A6" s="7">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="32" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="8"/>
@@ -903,7 +915,7 @@
       <c r="A9" s="7">
         <v>3</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="8"/>
@@ -922,7 +934,9 @@
         <v>7</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -945,7 +959,7 @@
       <c r="A12" s="7">
         <v>5</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="32" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="8"/>
@@ -959,7 +973,7 @@
       <c r="A13" s="7">
         <v>6</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="32" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="8"/>
@@ -974,7 +988,7 @@
         <v>6.1</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="7"/>
@@ -1071,7 +1085,7 @@
       <c r="A21" s="7">
         <v>7</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="8"/>
@@ -1086,7 +1100,7 @@
         <v>7.1</v>
       </c>
       <c r="B22" s="8"/>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="32" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="7"/>
@@ -1100,7 +1114,7 @@
         <v>7.2</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="32" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="7"/>
@@ -1114,7 +1128,7 @@
         <v>7.3</v>
       </c>
       <c r="B24" s="8"/>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="32" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="7"/>
@@ -1128,7 +1142,7 @@
         <v>7.4</v>
       </c>
       <c r="B25" s="8"/>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="32" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="7"/>
@@ -1237,7 +1251,7 @@
       <c r="A3" s="19">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="32" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="20"/>
@@ -1247,7 +1261,7 @@
       <c r="A4" s="19">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="32" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="20"/>
@@ -1257,7 +1271,7 @@
       <c r="A5" s="19">
         <v>2.1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="32" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="20"/>
@@ -1267,7 +1281,7 @@
       <c r="A6" s="19">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="32" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="20"/>
@@ -1277,7 +1291,7 @@
       <c r="A7" s="19">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="32" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="20"/>
@@ -1295,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,7 +1389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>

</xml_diff>